<commit_message>
Status code check 2.0
</commit_message>
<xml_diff>
--- a/error_log_report/failed_cases.xlsx
+++ b/error_log_report/failed_cases.xlsx
@@ -4,10 +4,8 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Sitegen" sheetId="1" r:id="rId1"/>
-    <sheet name="LMBC" sheetId="2" r:id="rId2"/>
-    <sheet name="Allerganpro" sheetId="3" r:id="rId3"/>
-    <sheet name="ADPA" sheetId="4" r:id="rId4"/>
-    <sheet name="Abbvie Pro Medical" sheetId="5" r:id="rId5"/>
+    <sheet name="Allerganpro" sheetId="2" r:id="rId2"/>
+    <sheet name="ADPA" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -401,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -417,6 +415,9 @@
         <v>errorMessage</v>
       </c>
       <c r="D1" t="str">
+        <v>statusCode</v>
+      </c>
+      <c r="E1" t="str">
         <v>timestamp</v>
       </c>
     </row>
@@ -434,19 +435,22 @@
 </v>
       </c>
       <c r="D2" t="str">
-        <v>2024-06-13T13:36:13.721Z</v>
+        <v>Unknown</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2024-06-21T06:14:14.947Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -462,36 +466,42 @@
         <v>errorMessage</v>
       </c>
       <c r="D1" t="str">
+        <v>statusCode</v>
+      </c>
+      <c r="E1" t="str">
         <v>timestamp</v>
       </c>
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>Sweden</v>
+        <v>India</v>
       </c>
       <c r="B2" t="str">
-        <v>https://www.let-me-be-clear.com/se/sv-se.html</v>
+        <v>https://www.allerganpro.com/in/en.html</v>
       </c>
       <c r="C2" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.goto: net::ERR_ABORTED; maybe frame was detached?
+        <v xml:space="preserve">page.goto: Test ended.
 Call log:
-  _x001b_[2m- navigating to "https://www.let-me-be-clear.com/se/sv-se.html", waiting until "load"_x001b_[22m
+  _x001b_[2m- navigating to "https://www.allerganpro.com/in/en.html", waiting until "load"_x001b_[22m
 </v>
       </c>
-      <c r="D2" t="str">
-        <v>2024-06-13T13:37:30.168Z</v>
+      <c r="D2">
+        <v>404</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2024-06-21T06:17:08.073Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -507,51 +517,9 @@
         <v>errorMessage</v>
       </c>
       <c r="D1" t="str">
-        <v>timestamp</v>
-      </c>
-    </row>
-    <row r="2" xml:space="preserve">
-      <c r="A2" t="str">
-        <v>India</v>
-      </c>
-      <c r="B2" t="str">
-        <v>https://www.allerganpro.com/in/en.html</v>
-      </c>
-      <c r="C2" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.goto: Test ended.
-Call log:
-  _x001b_[2m- navigating to "https://www.allerganpro.com/in/en.html", waiting until "load"_x001b_[22m
-</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2024-06-13T13:40:58.892Z</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>country</v>
-      </c>
-      <c r="B1" t="str">
-        <v>url</v>
-      </c>
-      <c r="C1" t="str">
-        <v>errorMessage</v>
-      </c>
-      <c r="D1" t="str">
+        <v>statusCode</v>
+      </c>
+      <c r="E1" t="str">
         <v>timestamp</v>
       </c>
     </row>
@@ -569,7 +537,10 @@
 </v>
       </c>
       <c r="D2" t="str">
-        <v>2024-06-13T13:41:48.662Z</v>
+        <v>Unknown</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2024-06-21T06:20:25.392Z</v>
       </c>
     </row>
     <row r="3" xml:space="preserve">
@@ -585,8 +556,11 @@
   _x001b_[2m- navigating to "https://www.lets-talk-eczema.com/py/es.html", waiting until "load"_x001b_[22m
 </v>
       </c>
-      <c r="D3" t="str">
-        <v>2024-06-13T13:42:14.847Z</v>
+      <c r="D3">
+        <v>404</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2024-06-21T06:20:42.174Z</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
@@ -602,75 +576,16 @@
   _x001b_[2m- navigating to "https://www.lets-talk-eczema.com/uy/es.html", waiting until "load"_x001b_[22m
 </v>
       </c>
-      <c r="D4" t="str">
-        <v>2024-06-13T13:42:47.386Z</v>
+      <c r="D4">
+        <v>404</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2024-06-21T06:20:58.782Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>country</v>
-      </c>
-      <c r="B1" t="str">
-        <v>url</v>
-      </c>
-      <c r="C1" t="str">
-        <v>errorMessage</v>
-      </c>
-      <c r="D1" t="str">
-        <v>timestamp</v>
-      </c>
-    </row>
-    <row r="2" xml:space="preserve">
-      <c r="A2" t="str">
-        <v>Medical Latvia</v>
-      </c>
-      <c r="B2" t="str">
-        <v>https://medical.abbviepro.com/bal/lav.html</v>
-      </c>
-      <c r="C2" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.goto: net::ERR_ABORTED; maybe frame was detached?
-Call log:
-  _x001b_[2m- navigating to "https://medical.abbviepro.com/bal/lav.html", waiting until "load"_x001b_[22m
-</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2024-06-13T13:44:52.707Z</v>
-      </c>
-    </row>
-    <row r="3" xml:space="preserve">
-      <c r="A3" t="str">
-        <v>Lithuania</v>
-      </c>
-      <c r="B3" t="str">
-        <v>https://medical.abbviepro.com/bal/lit.html</v>
-      </c>
-      <c r="C3" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.goto: net::ERR_ABORTED; maybe frame was detached?
-Call log:
-  _x001b_[2m- navigating to "https://medical.abbviepro.com/bal/lit.html", waiting until "load"_x001b_[22m
-</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2024-06-13T13:44:54.642Z</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>